<commit_message>
update server.py and train.js
</commit_message>
<xml_diff>
--- a/upload/Quangdohoi.xlsx
+++ b/upload/Quangdohoi.xlsx
@@ -5,27 +5,28 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="964" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t xml:space="preserve">Số thứ tự</t>
+    <t>Số thứ tự</t>
   </si>
   <si>
-    <t xml:space="preserve">Tiền</t>
+    <t>Số</t>
+  </si>
+  <si>
+    <t>quang</t>
+  </si>
+  <si>
+    <t>Tiền</t>
   </si>
 </sst>
 </file>
@@ -33,7 +34,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -126,13 +127,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B151"/>
+  <dimension ref="A1:D151"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B151"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.72959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="17.3622448979592"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.72959183673469"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -141,14 +147,26 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="n">
-        <f aca="true">2 * A2 + 3 + RAND()*(50-3) + 3</f>
-        <v>48.6829198952811</v>
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <f aca="true">2 * B2 + 3 + RAND()*(50-3) + 3</f>
+        <v>20.1119301351719</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -156,8 +174,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="n">
-        <f aca="true">2 * A3 + 3 + RAND()*(50-3) + 3</f>
-        <v>33.9552799541308</v>
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <f aca="true">2 * B3 + 3 + RAND()*(50-3) + 3</f>
+        <v>10.2723922866862</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -165,8 +189,14 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="n">
-        <f aca="true">2 * A4 + 3 + RAND()*(50-3) + 3</f>
-        <v>42.438523304511</v>
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <f aca="true">2 * B4 + 3 + RAND()*(50-3) + 3</f>
+        <v>53.9915455982555</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -174,8 +204,14 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="n">
-        <f aca="true">2 * A5 + 3 + RAND()*(50-3) + 3</f>
-        <v>48.7315297313177</v>
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <f aca="true">2 * B5 + 3 + RAND()*(50-3) + 3</f>
+        <v>32.6025987879839</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -183,8 +219,14 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="n">
-        <f aca="true">2 * A6 + 3 + RAND()*(50-3) + 3</f>
-        <v>40.5063721969366</v>
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <f aca="true">2 * B6 + 3 + RAND()*(50-3) + 3</f>
+        <v>22.2789913190063</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -192,8 +234,14 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="n">
-        <f aca="true">2 * A7 + 3 + RAND()*(50-3) + 3</f>
-        <v>30.8291066590475</v>
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="true">2 * B7 + 3 + RAND()*(50-3) + 3</f>
+        <v>64.7501077530906</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -201,8 +249,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="n">
-        <f aca="true">2 * A8 + 3 + RAND()*(50-3) + 3</f>
-        <v>60.3761736220266</v>
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <f aca="true">2 * B8 + 3 + RAND()*(50-3) + 3</f>
+        <v>61.8908535963856</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -210,8 +264,14 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="n">
-        <f aca="true">2 * A9 + 3 + RAND()*(50-3) + 3</f>
-        <v>52.2893254118867</v>
+        <v>8</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <f aca="true">2 * B9 + 3 + RAND()*(50-3) + 3</f>
+        <v>50.8315814463422</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -219,8 +279,14 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="n">
-        <f aca="true">2 * A10 + 3 + RAND()*(50-3) + 3</f>
-        <v>36.1695342664806</v>
+        <v>9</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <f aca="true">2 * B10 + 3 + RAND()*(50-3) + 3</f>
+        <v>35.892719098134</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -228,8 +294,14 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="n">
-        <f aca="true">2 * A11 + 3 + RAND()*(50-3) + 3</f>
-        <v>58.2303530815181</v>
+        <v>10</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <f aca="true">2 * B11 + 3 + RAND()*(50-3) + 3</f>
+        <v>46.8732026668731</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -237,8 +309,14 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="n">
-        <f aca="true">2 * A12 + 3 + RAND()*(50-3) + 3</f>
-        <v>60.6357232158496</v>
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <f aca="true">2 * B12 + 3 + RAND()*(50-3) + 3</f>
+        <v>50.7258551355917</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -246,8 +324,14 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="n">
-        <f aca="true">2 * A13 + 3 + RAND()*(50-3) + 3</f>
-        <v>54.2527059576647</v>
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <f aca="true">2 * B13 + 3 + RAND()*(50-3) + 3</f>
+        <v>72.3019250733778</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -255,8 +339,14 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="n">
-        <f aca="true">2 * A14 + 3 + RAND()*(50-3) + 3</f>
-        <v>64.9357041565941</v>
+        <v>13</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <f aca="true">2 * B14 + 3 + RAND()*(50-3) + 3</f>
+        <v>32.2572775515728</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -264,8 +354,14 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="n">
-        <f aca="true">2 * A15 + 3 + RAND()*(50-3) + 3</f>
-        <v>64.5352801196072</v>
+        <v>14</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <f aca="true">2 * B15 + 3 + RAND()*(50-3) + 3</f>
+        <v>41.437403427437</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -273,8 +369,14 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="n">
-        <f aca="true">2 * A16 + 3 + RAND()*(50-3) + 3</f>
-        <v>59.0516089368274</v>
+        <v>15</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <f aca="true">2 * B16 + 3 + RAND()*(50-3) + 3</f>
+        <v>79.4147881884128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -282,8 +384,14 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="n">
-        <f aca="true">2 * A17 + 3 + RAND()*(50-3) + 3</f>
-        <v>64.3609944299458</v>
+        <v>16</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <f aca="true">2 * B17 + 3 + RAND()*(50-3) + 3</f>
+        <v>60.6806136197411</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -291,8 +399,14 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="n">
-        <f aca="true">2 * A18 + 3 + RAND()*(50-3) + 3</f>
-        <v>79.5578859362249</v>
+        <v>17</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1" t="n">
+        <f aca="true">2 * B18 + 3 + RAND()*(50-3) + 3</f>
+        <v>66.9145232436713</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,8 +414,14 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="n">
-        <f aca="true">2 * A19 + 3 + RAND()*(50-3) + 3</f>
-        <v>87.0916437507706</v>
+        <v>18</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1" t="n">
+        <f aca="true">2 * B19 + 3 + RAND()*(50-3) + 3</f>
+        <v>86.4267124265898</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -309,8 +429,14 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="n">
-        <f aca="true">2 * A20 + 3 + RAND()*(50-3) + 3</f>
-        <v>69.950354863389</v>
+        <v>19</v>
+      </c>
+      <c r="C20" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="D20" s="1" t="n">
+        <f aca="true">2 * B20 + 3 + RAND()*(50-3) + 3</f>
+        <v>83.4520206197631</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -318,8 +444,14 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="n">
-        <f aca="true">2 * A21 + 3 + RAND()*(50-3) + 3</f>
-        <v>72.0388952909676</v>
+        <v>20</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <f aca="true">2 * B21 + 3 + RAND()*(50-3) + 3</f>
+        <v>80.49749024841</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -327,8 +459,14 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="n">
-        <f aca="true">2 * A22 + 3 + RAND()*(50-3) + 3</f>
-        <v>80.5453985310812</v>
+        <v>21</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <f aca="true">2 * B22 + 3 + RAND()*(50-3) + 3</f>
+        <v>71.0693324815948</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,8 +474,14 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="n">
-        <f aca="true">2 * A23 + 3 + RAND()*(50-3) + 3</f>
-        <v>96.1069950485304</v>
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="true">2 * B23 + 3 + RAND()*(50-3) + 3</f>
+        <v>91.3059516076464</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -345,8 +489,14 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="n">
-        <f aca="true">2 * A24 + 3 + RAND()*(50-3) + 3</f>
-        <v>78.6624671577087</v>
+        <v>23</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="true">2 * B24 + 3 + RAND()*(50-3) + 3</f>
+        <v>55.7196031357162</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -354,8 +504,14 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="n">
-        <f aca="true">2 * A25 + 3 + RAND()*(50-3) + 3</f>
-        <v>82.0354739762872</v>
+        <v>24</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <f aca="true">2 * B25 + 3 + RAND()*(50-3) + 3</f>
+        <v>67.7361165015027</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -363,8 +519,14 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="n">
-        <f aca="true">2 * A26 + 3 + RAND()*(50-3) + 3</f>
-        <v>100.878412145081</v>
+        <v>25</v>
+      </c>
+      <c r="C26" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="D26" s="1" t="n">
+        <f aca="true">2 * B26 + 3 + RAND()*(50-3) + 3</f>
+        <v>56.4756797556765</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -372,8 +534,14 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="n">
-        <f aca="true">2 * A27 + 3 + RAND()*(50-3) + 3</f>
-        <v>79.1157514674585</v>
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="D27" s="1" t="n">
+        <f aca="true">2 * B27 + 3 + RAND()*(50-3) + 3</f>
+        <v>102.149519657949</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -381,8 +549,14 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="n">
-        <f aca="true">2 * A28 + 3 + RAND()*(50-3) + 3</f>
-        <v>79.1912598973044</v>
+        <v>27</v>
+      </c>
+      <c r="C28" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="n">
+        <f aca="true">2 * B28 + 3 + RAND()*(50-3) + 3</f>
+        <v>81.4722537768539</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -390,8 +564,14 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="n">
-        <f aca="true">2 * A29 + 3 + RAND()*(50-3) + 3</f>
-        <v>107.581424576214</v>
+        <v>28</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="true">2 * B29 + 3 + RAND()*(50-3) + 3</f>
+        <v>90.4514714085963</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -399,8 +579,14 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="n">
-        <f aca="true">2 * A30 + 3 + RAND()*(50-3) + 3</f>
-        <v>78.3370201747459</v>
+        <v>29</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="true">2 * B30 + 3 + RAND()*(50-3) + 3</f>
+        <v>98.2106178791728</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -408,8 +594,14 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="n">
-        <f aca="true">2 * A31 + 3 + RAND()*(50-3) + 3</f>
-        <v>107.945416602903</v>
+        <v>30</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="true">2 * B31 + 3 + RAND()*(50-3) + 3</f>
+        <v>111.12094239099</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -417,8 +609,14 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="n">
-        <f aca="true">2 * A32 + 3 + RAND()*(50-3) + 3</f>
-        <v>80.8451095623331</v>
+        <v>31</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <f aca="true">2 * B32 + 3 + RAND()*(50-3) + 3</f>
+        <v>105.610491817119</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -426,8 +624,14 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="n">
-        <f aca="true">2 * A33 + 3 + RAND()*(50-3) + 3</f>
-        <v>84.1209648065372</v>
+        <v>32</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <f aca="true">2 * B33 + 3 + RAND()*(50-3) + 3</f>
+        <v>83.31744653848</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -435,8 +639,14 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="n">
-        <f aca="true">2 * A34 + 3 + RAND()*(50-3) + 3</f>
-        <v>79.4980368796895</v>
+        <v>33</v>
+      </c>
+      <c r="C34" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1" t="n">
+        <f aca="true">2 * B34 + 3 + RAND()*(50-3) + 3</f>
+        <v>111.435500349617</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -444,8 +654,14 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="n">
-        <f aca="true">2 * A35 + 3 + RAND()*(50-3) + 3</f>
-        <v>87.0562178748044</v>
+        <v>34</v>
+      </c>
+      <c r="C35" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="true">2 * B35 + 3 + RAND()*(50-3) + 3</f>
+        <v>90.076940436149</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -453,8 +669,14 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="n">
-        <f aca="true">2 * A36 + 3 + RAND()*(50-3) + 3</f>
-        <v>83.7460909157988</v>
+        <v>35</v>
+      </c>
+      <c r="C36" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="true">2 * B36 + 3 + RAND()*(50-3) + 3</f>
+        <v>101.899603162194</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -462,8 +684,14 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="n">
-        <f aca="true">2 * A37 + 3 + RAND()*(50-3) + 3</f>
-        <v>78.047757475387</v>
+        <v>36</v>
+      </c>
+      <c r="C37" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <f aca="true">2 * B37 + 3 + RAND()*(50-3) + 3</f>
+        <v>93.2902444079518</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -471,8 +699,14 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="n">
-        <f aca="true">2 * A38 + 3 + RAND()*(50-3) + 3</f>
-        <v>91.4322003258682</v>
+        <v>37</v>
+      </c>
+      <c r="C38" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <f aca="true">2 * B38 + 3 + RAND()*(50-3) + 3</f>
+        <v>88.2677488029003</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -480,8 +714,14 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="n">
-        <f aca="true">2 * A39 + 3 + RAND()*(50-3) + 3</f>
-        <v>111.646314594249</v>
+        <v>38</v>
+      </c>
+      <c r="C39" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <f aca="true">2 * B39 + 3 + RAND()*(50-3) + 3</f>
+        <v>117.442075864645</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -489,8 +729,14 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="n">
-        <f aca="true">2 * A40 + 3 + RAND()*(50-3) + 3</f>
-        <v>113.60870384248</v>
+        <v>39</v>
+      </c>
+      <c r="C40" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="D40" s="1" t="n">
+        <f aca="true">2 * B40 + 3 + RAND()*(50-3) + 3</f>
+        <v>112.20445702807</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -498,8 +744,14 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="n">
-        <f aca="true">2 * A41 + 3 + RAND()*(50-3) + 3</f>
-        <v>100.448686315621</v>
+        <v>40</v>
+      </c>
+      <c r="C41" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="D41" s="1" t="n">
+        <f aca="true">2 * B41 + 3 + RAND()*(50-3) + 3</f>
+        <v>132.280487344833</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,8 +759,14 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="n">
-        <f aca="true">2 * A42 + 3 + RAND()*(50-3) + 3</f>
-        <v>107.079273386096</v>
+        <v>41</v>
+      </c>
+      <c r="C42" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="D42" s="1" t="n">
+        <f aca="true">2 * B42 + 3 + RAND()*(50-3) + 3</f>
+        <v>104.294111154275</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -516,8 +774,14 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="n">
-        <f aca="true">2 * A43 + 3 + RAND()*(50-3) + 3</f>
-        <v>118.247108773804</v>
+        <v>42</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <f aca="true">2 * B43 + 3 + RAND()*(50-3) + 3</f>
+        <v>125.414107729914</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -525,8 +789,14 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="n">
-        <f aca="true">2 * A44 + 3 + RAND()*(50-3) + 3</f>
-        <v>111.872543254279</v>
+        <v>43</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <f aca="true">2 * B44 + 3 + RAND()*(50-3) + 3</f>
+        <v>116.481820076704</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -534,8 +804,14 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="n">
-        <f aca="true">2 * A45 + 3 + RAND()*(50-3) + 3</f>
-        <v>116.728158114954</v>
+        <v>44</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <f aca="true">2 * B45 + 3 + RAND()*(50-3) + 3</f>
+        <v>110.283194585238</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -543,8 +819,14 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="n">
-        <f aca="true">2 * A46 + 3 + RAND()*(50-3) + 3</f>
-        <v>140.646250440178</v>
+        <v>45</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <f aca="true">2 * B46 + 3 + RAND()*(50-3) + 3</f>
+        <v>142.88494910975</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,8 +834,14 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="n">
-        <f aca="true">2 * A47 + 3 + RAND()*(50-3) + 3</f>
-        <v>142.529061647953</v>
+        <v>46</v>
+      </c>
+      <c r="C47" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="D47" s="1" t="n">
+        <f aca="true">2 * B47 + 3 + RAND()*(50-3) + 3</f>
+        <v>99.0161627731286</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -561,8 +849,14 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="n">
-        <f aca="true">2 * A48 + 3 + RAND()*(50-3) + 3</f>
-        <v>108.832181915229</v>
+        <v>47</v>
+      </c>
+      <c r="C48" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="D48" s="1" t="n">
+        <f aca="true">2 * B48 + 3 + RAND()*(50-3) + 3</f>
+        <v>108.704219229519</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -570,8 +864,14 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="n">
-        <f aca="true">2 * A49 + 3 + RAND()*(50-3) + 3</f>
-        <v>113.121347892084</v>
+        <v>48</v>
+      </c>
+      <c r="C49" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="D49" s="1" t="n">
+        <f aca="true">2 * B49 + 3 + RAND()*(50-3) + 3</f>
+        <v>126.826922595501</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -579,8 +879,14 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="n">
-        <f aca="true">2 * A50 + 3 + RAND()*(50-3) + 3</f>
-        <v>150.075015814079</v>
+        <v>49</v>
+      </c>
+      <c r="C50" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="D50" s="1" t="n">
+        <f aca="true">2 * B50 + 3 + RAND()*(50-3) + 3</f>
+        <v>150.81626400142</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -588,8 +894,14 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="n">
-        <f aca="true">2 * A51 + 3 + RAND()*(50-3) + 3</f>
-        <v>149.173987318805</v>
+        <v>50</v>
+      </c>
+      <c r="C51" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="D51" s="1" t="n">
+        <f aca="true">2 * B51 + 3 + RAND()*(50-3) + 3</f>
+        <v>108.086403195048</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -597,8 +909,14 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="n">
-        <f aca="true">2 * A52 + 3 + RAND()*(50-3) + 3</f>
-        <v>129.170766074623</v>
+        <v>51</v>
+      </c>
+      <c r="C52" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <f aca="true">2 * B52 + 3 + RAND()*(50-3) + 3</f>
+        <v>133.493416023673</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -606,8 +924,14 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="n">
-        <f aca="true">2 * A53 + 3 + RAND()*(50-3) + 3</f>
-        <v>150.899409364601</v>
+        <v>52</v>
+      </c>
+      <c r="C53" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <f aca="true">2 * B53 + 3 + RAND()*(50-3) + 3</f>
+        <v>119.847200556891</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -615,8 +939,14 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="n">
-        <f aca="true">2 * A54 + 3 + RAND()*(50-3) + 3</f>
-        <v>124.894564556838</v>
+        <v>53</v>
+      </c>
+      <c r="C54" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <f aca="true">2 * B54 + 3 + RAND()*(50-3) + 3</f>
+        <v>128.42494483036</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -624,8 +954,14 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="n">
-        <f aca="true">2 * A55 + 3 + RAND()*(50-3) + 3</f>
-        <v>144.863547287734</v>
+        <v>54</v>
+      </c>
+      <c r="C55" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <f aca="true">2 * B55 + 3 + RAND()*(50-3) + 3</f>
+        <v>138.074106953107</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -633,8 +969,14 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="n">
-        <f aca="true">2 * A56 + 3 + RAND()*(50-3) + 3</f>
-        <v>135.413911979951</v>
+        <v>55</v>
+      </c>
+      <c r="C56" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <f aca="true">2 * B56 + 3 + RAND()*(50-3) + 3</f>
+        <v>155.824354390847</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,8 +984,14 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="n">
-        <f aca="true">2 * A57 + 3 + RAND()*(50-3) + 3</f>
-        <v>143.108830799467</v>
+        <v>56</v>
+      </c>
+      <c r="C57" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="D57" s="1" t="n">
+        <f aca="true">2 * B57 + 3 + RAND()*(50-3) + 3</f>
+        <v>122.721889794571</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -651,8 +999,14 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="n">
-        <f aca="true">2 * A58 + 3 + RAND()*(50-3) + 3</f>
-        <v>136.744508484267</v>
+        <v>57</v>
+      </c>
+      <c r="C58" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="D58" s="1" t="n">
+        <f aca="true">2 * B58 + 3 + RAND()*(50-3) + 3</f>
+        <v>153.35691428883</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -660,8 +1014,14 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="n">
-        <f aca="true">2 * A59 + 3 + RAND()*(50-3) + 3</f>
-        <v>162.829543553609</v>
+        <v>58</v>
+      </c>
+      <c r="C59" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <f aca="true">2 * B59 + 3 + RAND()*(50-3) + 3</f>
+        <v>163.547374411952</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -669,8 +1029,14 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="n">
-        <f aca="true">2 * A60 + 3 + RAND()*(50-3) + 3</f>
-        <v>167.950788918642</v>
+        <v>59</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="D60" s="1" t="n">
+        <f aca="true">2 * B60 + 3 + RAND()*(50-3) + 3</f>
+        <v>150.228833348257</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,8 +1044,14 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="n">
-        <f aca="true">2 * A61 + 3 + RAND()*(50-3) + 3</f>
-        <v>157.313461765038</v>
+        <v>60</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <f aca="true">2 * B61 + 3 + RAND()*(50-3) + 3</f>
+        <v>147.756360719446</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -687,8 +1059,14 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="n">
-        <f aca="true">2 * A62 + 3 + RAND()*(50-3) + 3</f>
-        <v>156.122313195808</v>
+        <v>61</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="D62" s="1" t="n">
+        <f aca="true">2 * B62 + 3 + RAND()*(50-3) + 3</f>
+        <v>136.891465700697</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -696,8 +1074,14 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="n">
-        <f aca="true">2 * A63 + 3 + RAND()*(50-3) + 3</f>
-        <v>167.973576668873</v>
+        <v>62</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <f aca="true">2 * B63 + 3 + RAND()*(50-3) + 3</f>
+        <v>170.902960974956</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,8 +1089,14 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="n">
-        <f aca="true">2 * A64 + 3 + RAND()*(50-3) + 3</f>
-        <v>143.324578037579</v>
+        <v>63</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="D64" s="1" t="n">
+        <f aca="true">2 * B64 + 3 + RAND()*(50-3) + 3</f>
+        <v>139.615866193781</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -714,8 +1104,14 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="n">
-        <f aca="true">2 * A65 + 3 + RAND()*(50-3) + 3</f>
-        <v>177.077376410791</v>
+        <v>64</v>
+      </c>
+      <c r="C65" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="D65" s="1" t="n">
+        <f aca="true">2 * B65 + 3 + RAND()*(50-3) + 3</f>
+        <v>141.840516348602</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,8 +1119,14 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="n">
-        <f aca="true">2 * A66 + 3 + RAND()*(50-3) + 3</f>
-        <v>174.517623656417</v>
+        <v>65</v>
+      </c>
+      <c r="C66" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <f aca="true">2 * B66 + 3 + RAND()*(50-3) + 3</f>
+        <v>138.486530570313</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,8 +1134,14 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="n">
-        <f aca="true">2 * A67 + 3 + RAND()*(50-3) + 3</f>
-        <v>142.559907398492</v>
+        <v>66</v>
+      </c>
+      <c r="C67" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="D67" s="1" t="n">
+        <f aca="true">2 * B67 + 3 + RAND()*(50-3) + 3</f>
+        <v>171.089399873279</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -741,8 +1149,14 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="n">
-        <f aca="true">2 * A68 + 3 + RAND()*(50-3) + 3</f>
-        <v>186.695313712511</v>
+        <v>67</v>
+      </c>
+      <c r="C68" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="D68" s="1" t="n">
+        <f aca="true">2 * B68 + 3 + RAND()*(50-3) + 3</f>
+        <v>154.903805922484</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -750,8 +1164,14 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="n">
-        <f aca="true">2 * A69 + 3 + RAND()*(50-3) + 3</f>
-        <v>148.671560292875</v>
+        <v>68</v>
+      </c>
+      <c r="C69" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="D69" s="1" t="n">
+        <f aca="true">2 * B69 + 3 + RAND()*(50-3) + 3</f>
+        <v>152.20708144363</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -759,8 +1179,14 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="n">
-        <f aca="true">2 * A70 + 3 + RAND()*(50-3) + 3</f>
-        <v>161.653789633413</v>
+        <v>69</v>
+      </c>
+      <c r="C70" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="D70" s="1" t="n">
+        <f aca="true">2 * B70 + 3 + RAND()*(50-3) + 3</f>
+        <v>151.400086018723</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -768,8 +1194,14 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="n">
-        <f aca="true">2 * A71 + 3 + RAND()*(50-3) + 3</f>
-        <v>149.678552333675</v>
+        <v>70</v>
+      </c>
+      <c r="C71" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="D71" s="1" t="n">
+        <f aca="true">2 * B71 + 3 + RAND()*(50-3) + 3</f>
+        <v>181.554343797499</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -777,8 +1209,14 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="n">
-        <f aca="true">2 * A72 + 3 + RAND()*(50-3) + 3</f>
-        <v>168.871674725809</v>
+        <v>71</v>
+      </c>
+      <c r="C72" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="D72" s="1" t="n">
+        <f aca="true">2 * B72 + 3 + RAND()*(50-3) + 3</f>
+        <v>187.640133046545</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,8 +1224,14 @@
         <v>72</v>
       </c>
       <c r="B73" s="1" t="n">
-        <f aca="true">2 * A73 + 3 + RAND()*(50-3) + 3</f>
-        <v>153.182522040958</v>
+        <v>72</v>
+      </c>
+      <c r="C73" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="D73" s="1" t="n">
+        <f aca="true">2 * B73 + 3 + RAND()*(50-3) + 3</f>
+        <v>174.196436726954</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -795,8 +1239,14 @@
         <v>73</v>
       </c>
       <c r="B74" s="1" t="n">
-        <f aca="true">2 * A74 + 3 + RAND()*(50-3) + 3</f>
-        <v>175.747541368835</v>
+        <v>73</v>
+      </c>
+      <c r="C74" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="D74" s="1" t="n">
+        <f aca="true">2 * B74 + 3 + RAND()*(50-3) + 3</f>
+        <v>189.755347281229</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -804,8 +1254,14 @@
         <v>74</v>
       </c>
       <c r="B75" s="1" t="n">
-        <f aca="true">2 * A75 + 3 + RAND()*(50-3) + 3</f>
-        <v>158.923141587701</v>
+        <v>74</v>
+      </c>
+      <c r="C75" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="D75" s="1" t="n">
+        <f aca="true">2 * B75 + 3 + RAND()*(50-3) + 3</f>
+        <v>165.133584298659</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -813,8 +1269,14 @@
         <v>75</v>
       </c>
       <c r="B76" s="1" t="n">
-        <f aca="true">2 * A76 + 3 + RAND()*(50-3) + 3</f>
-        <v>174.983500701437</v>
+        <v>75</v>
+      </c>
+      <c r="C76" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="D76" s="1" t="n">
+        <f aca="true">2 * B76 + 3 + RAND()*(50-3) + 3</f>
+        <v>165.253355499823</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,8 +1284,14 @@
         <v>76</v>
       </c>
       <c r="B77" s="1" t="n">
-        <f aca="true">2 * A77 + 3 + RAND()*(50-3) + 3</f>
-        <v>177.141204904194</v>
+        <v>76</v>
+      </c>
+      <c r="C77" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="D77" s="1" t="n">
+        <f aca="true">2 * B77 + 3 + RAND()*(50-3) + 3</f>
+        <v>192.466247693403</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,8 +1299,14 @@
         <v>77</v>
       </c>
       <c r="B78" s="1" t="n">
-        <f aca="true">2 * A78 + 3 + RAND()*(50-3) + 3</f>
-        <v>170.479028905568</v>
+        <v>77</v>
+      </c>
+      <c r="C78" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="D78" s="1" t="n">
+        <f aca="true">2 * B78 + 3 + RAND()*(50-3) + 3</f>
+        <v>161.349801483331</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,8 +1314,14 @@
         <v>78</v>
       </c>
       <c r="B79" s="1" t="n">
-        <f aca="true">2 * A79 + 3 + RAND()*(50-3) + 3</f>
-        <v>192.450665195037</v>
+        <v>78</v>
+      </c>
+      <c r="C79" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="D79" s="1" t="n">
+        <f aca="true">2 * B79 + 3 + RAND()*(50-3) + 3</f>
+        <v>171.957841095515</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -849,8 +1329,14 @@
         <v>79</v>
       </c>
       <c r="B80" s="1" t="n">
-        <f aca="true">2 * A80 + 3 + RAND()*(50-3) + 3</f>
-        <v>168.908556460158</v>
+        <v>79</v>
+      </c>
+      <c r="C80" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="D80" s="1" t="n">
+        <f aca="true">2 * B80 + 3 + RAND()*(50-3) + 3</f>
+        <v>164.202051627683</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -858,8 +1344,14 @@
         <v>80</v>
       </c>
       <c r="B81" s="1" t="n">
-        <f aca="true">2 * A81 + 3 + RAND()*(50-3) + 3</f>
-        <v>192.045550846918</v>
+        <v>80</v>
+      </c>
+      <c r="C81" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="D81" s="1" t="n">
+        <f aca="true">2 * B81 + 3 + RAND()*(50-3) + 3</f>
+        <v>212.718241510447</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -867,8 +1359,14 @@
         <v>81</v>
       </c>
       <c r="B82" s="1" t="n">
-        <f aca="true">2 * A82 + 3 + RAND()*(50-3) + 3</f>
-        <v>204.587359028536</v>
+        <v>81</v>
+      </c>
+      <c r="C82" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="D82" s="1" t="n">
+        <f aca="true">2 * B82 + 3 + RAND()*(50-3) + 3</f>
+        <v>195.42864672048</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -876,8 +1374,14 @@
         <v>82</v>
       </c>
       <c r="B83" s="1" t="n">
-        <f aca="true">2 * A83 + 3 + RAND()*(50-3) + 3</f>
-        <v>215.534343385044</v>
+        <v>82</v>
+      </c>
+      <c r="C83" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="D83" s="1" t="n">
+        <f aca="true">2 * B83 + 3 + RAND()*(50-3) + 3</f>
+        <v>180.900691101793</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -885,8 +1389,14 @@
         <v>83</v>
       </c>
       <c r="B84" s="1" t="n">
-        <f aca="true">2 * A84 + 3 + RAND()*(50-3) + 3</f>
-        <v>189.533244201292</v>
+        <v>83</v>
+      </c>
+      <c r="C84" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="D84" s="1" t="n">
+        <f aca="true">2 * B84 + 3 + RAND()*(50-3) + 3</f>
+        <v>172.67188425432</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -894,8 +1404,14 @@
         <v>84</v>
       </c>
       <c r="B85" s="1" t="n">
-        <f aca="true">2 * A85 + 3 + RAND()*(50-3) + 3</f>
-        <v>175.046949477844</v>
+        <v>84</v>
+      </c>
+      <c r="C85" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="D85" s="1" t="n">
+        <f aca="true">2 * B85 + 3 + RAND()*(50-3) + 3</f>
+        <v>210.615971083753</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,8 +1419,14 @@
         <v>85</v>
       </c>
       <c r="B86" s="1" t="n">
-        <f aca="true">2 * A86 + 3 + RAND()*(50-3) + 3</f>
-        <v>193.031184246549</v>
+        <v>85</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="D86" s="1" t="n">
+        <f aca="true">2 * B86 + 3 + RAND()*(50-3) + 3</f>
+        <v>192.968227887293</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,8 +1434,14 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="n">
-        <f aca="true">2 * A87 + 3 + RAND()*(50-3) + 3</f>
-        <v>215.164148279692</v>
+        <v>86</v>
+      </c>
+      <c r="C87" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="D87" s="1" t="n">
+        <f aca="true">2 * B87 + 3 + RAND()*(50-3) + 3</f>
+        <v>220.688723650528</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -921,8 +1449,14 @@
         <v>87</v>
       </c>
       <c r="B88" s="1" t="n">
-        <f aca="true">2 * A88 + 3 + RAND()*(50-3) + 3</f>
-        <v>180.72256669353</v>
+        <v>87</v>
+      </c>
+      <c r="C88" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="D88" s="1" t="n">
+        <f aca="true">2 * B88 + 3 + RAND()*(50-3) + 3</f>
+        <v>218.204997133464</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -930,8 +1464,14 @@
         <v>88</v>
       </c>
       <c r="B89" s="1" t="n">
-        <f aca="true">2 * A89 + 3 + RAND()*(50-3) + 3</f>
-        <v>204.721986532274</v>
+        <v>88</v>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="D89" s="1" t="n">
+        <f aca="true">2 * B89 + 3 + RAND()*(50-3) + 3</f>
+        <v>203.044405710883</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -939,8 +1479,14 @@
         <v>89</v>
       </c>
       <c r="B90" s="1" t="n">
-        <f aca="true">2 * A90 + 3 + RAND()*(50-3) + 3</f>
-        <v>228.626671075823</v>
+        <v>89</v>
+      </c>
+      <c r="C90" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="D90" s="1" t="n">
+        <f aca="true">2 * B90 + 3 + RAND()*(50-3) + 3</f>
+        <v>192.992570277071</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -948,8 +1494,14 @@
         <v>90</v>
       </c>
       <c r="B91" s="1" t="n">
-        <f aca="true">2 * A91 + 3 + RAND()*(50-3) + 3</f>
-        <v>186.116630630282</v>
+        <v>90</v>
+      </c>
+      <c r="C91" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="D91" s="1" t="n">
+        <f aca="true">2 * B91 + 3 + RAND()*(50-3) + 3</f>
+        <v>193.42208160623</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -957,8 +1509,14 @@
         <v>91</v>
       </c>
       <c r="B92" s="1" t="n">
-        <f aca="true">2 * A92 + 3 + RAND()*(50-3) + 3</f>
-        <v>210.124188903128</v>
+        <v>91</v>
+      </c>
+      <c r="C92" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="D92" s="1" t="n">
+        <f aca="true">2 * B92 + 3 + RAND()*(50-3) + 3</f>
+        <v>197.820713081164</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,8 +1524,14 @@
         <v>92</v>
       </c>
       <c r="B93" s="1" t="n">
-        <f aca="true">2 * A93 + 3 + RAND()*(50-3) + 3</f>
-        <v>204.460610601932</v>
+        <v>92</v>
+      </c>
+      <c r="C93" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="D93" s="1" t="n">
+        <f aca="true">2 * B93 + 3 + RAND()*(50-3) + 3</f>
+        <v>217.449045433896</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,8 +1539,14 @@
         <v>93</v>
       </c>
       <c r="B94" s="1" t="n">
-        <f aca="true">2 * A94 + 3 + RAND()*(50-3) + 3</f>
-        <v>198.166699656712</v>
+        <v>93</v>
+      </c>
+      <c r="C94" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="D94" s="1" t="n">
+        <f aca="true">2 * B94 + 3 + RAND()*(50-3) + 3</f>
+        <v>205.042135896161</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -984,8 +1554,14 @@
         <v>94</v>
       </c>
       <c r="B95" s="1" t="n">
-        <f aca="true">2 * A95 + 3 + RAND()*(50-3) + 3</f>
-        <v>228.718991106836</v>
+        <v>94</v>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="D95" s="1" t="n">
+        <f aca="true">2 * B95 + 3 + RAND()*(50-3) + 3</f>
+        <v>216.667004690738</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -993,8 +1569,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="1" t="n">
-        <f aca="true">2 * A96 + 3 + RAND()*(50-3) + 3</f>
-        <v>220.280146224288</v>
+        <v>95</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="D96" s="1" t="n">
+        <f aca="true">2 * B96 + 3 + RAND()*(50-3) + 3</f>
+        <v>222.693344308762</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1002,8 +1584,14 @@
         <v>96</v>
       </c>
       <c r="B97" s="1" t="n">
-        <f aca="true">2 * A97 + 3 + RAND()*(50-3) + 3</f>
-        <v>240.695803820359</v>
+        <v>96</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="D97" s="1" t="n">
+        <f aca="true">2 * B97 + 3 + RAND()*(50-3) + 3</f>
+        <v>200.079458325868</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1011,8 +1599,14 @@
         <v>97</v>
       </c>
       <c r="B98" s="1" t="n">
-        <f aca="true">2 * A98 + 3 + RAND()*(50-3) + 3</f>
-        <v>201.077922567473</v>
+        <v>97</v>
+      </c>
+      <c r="C98" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="D98" s="1" t="n">
+        <f aca="true">2 * B98 + 3 + RAND()*(50-3) + 3</f>
+        <v>239.741678244434</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1020,8 +1614,14 @@
         <v>98</v>
       </c>
       <c r="B99" s="1" t="n">
-        <f aca="true">2 * A99 + 3 + RAND()*(50-3) + 3</f>
-        <v>218.698252461868</v>
+        <v>98</v>
+      </c>
+      <c r="C99" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="D99" s="1" t="n">
+        <f aca="true">2 * B99 + 3 + RAND()*(50-3) + 3</f>
+        <v>218.82688555494</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1029,8 +1629,14 @@
         <v>99</v>
       </c>
       <c r="B100" s="1" t="n">
-        <f aca="true">2 * A100 + 3 + RAND()*(50-3) + 3</f>
-        <v>204.07245190874</v>
+        <v>99</v>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="D100" s="1" t="n">
+        <f aca="true">2 * B100 + 3 + RAND()*(50-3) + 3</f>
+        <v>217.338257071329</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,8 +1644,14 @@
         <v>100</v>
       </c>
       <c r="B101" s="1" t="n">
-        <f aca="true">2 * A101 + 3 + RAND()*(50-3) + 3</f>
-        <v>245.562115321667</v>
+        <v>100</v>
+      </c>
+      <c r="C101" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="D101" s="1" t="n">
+        <f aca="true">2 * B101 + 3 + RAND()*(50-3) + 3</f>
+        <v>208.298629081575</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1047,8 +1659,14 @@
         <v>101</v>
       </c>
       <c r="B102" s="1" t="n">
-        <f aca="true">2 * A102 + 3 + RAND()*(50-3) + 3</f>
-        <v>252.298085892726</v>
+        <v>101</v>
+      </c>
+      <c r="C102" s="1" t="n">
+        <v>101</v>
+      </c>
+      <c r="D102" s="1" t="n">
+        <f aca="true">2 * B102 + 3 + RAND()*(50-3) + 3</f>
+        <v>210.25875592581</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,8 +1674,14 @@
         <v>102</v>
       </c>
       <c r="B103" s="1" t="n">
-        <f aca="true">2 * A103 + 3 + RAND()*(50-3) + 3</f>
-        <v>243.923792985112</v>
+        <v>102</v>
+      </c>
+      <c r="C103" s="1" t="n">
+        <v>102</v>
+      </c>
+      <c r="D103" s="1" t="n">
+        <f aca="true">2 * B103 + 3 + RAND()*(50-3) + 3</f>
+        <v>235.610535980202</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1065,8 +1689,14 @@
         <v>103</v>
       </c>
       <c r="B104" s="1" t="n">
-        <f aca="true">2 * A104 + 3 + RAND()*(50-3) + 3</f>
-        <v>218.860784384076</v>
+        <v>103</v>
+      </c>
+      <c r="C104" s="1" t="n">
+        <v>103</v>
+      </c>
+      <c r="D104" s="1" t="n">
+        <f aca="true">2 * B104 + 3 + RAND()*(50-3) + 3</f>
+        <v>218.963248847052</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,8 +1704,14 @@
         <v>104</v>
       </c>
       <c r="B105" s="1" t="n">
-        <f aca="true">2 * A105 + 3 + RAND()*(50-3) + 3</f>
-        <v>215.410190036421</v>
+        <v>104</v>
+      </c>
+      <c r="C105" s="1" t="n">
+        <v>104</v>
+      </c>
+      <c r="D105" s="1" t="n">
+        <f aca="true">2 * B105 + 3 + RAND()*(50-3) + 3</f>
+        <v>253.338841733523</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1083,8 +1719,14 @@
         <v>105</v>
       </c>
       <c r="B106" s="1" t="n">
-        <f aca="true">2 * A106 + 3 + RAND()*(50-3) + 3</f>
-        <v>236.519287887383</v>
+        <v>105</v>
+      </c>
+      <c r="C106" s="1" t="n">
+        <v>105</v>
+      </c>
+      <c r="D106" s="1" t="n">
+        <f aca="true">2 * B106 + 3 + RAND()*(50-3) + 3</f>
+        <v>239.774499084568</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1092,8 +1734,14 @@
         <v>106</v>
       </c>
       <c r="B107" s="1" t="n">
-        <f aca="true">2 * A107 + 3 + RAND()*(50-3) + 3</f>
-        <v>255.446726505575</v>
+        <v>106</v>
+      </c>
+      <c r="C107" s="1" t="n">
+        <v>106</v>
+      </c>
+      <c r="D107" s="1" t="n">
+        <f aca="true">2 * B107 + 3 + RAND()*(50-3) + 3</f>
+        <v>235.038038027706</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1101,8 +1749,14 @@
         <v>107</v>
       </c>
       <c r="B108" s="1" t="n">
-        <f aca="true">2 * A108 + 3 + RAND()*(50-3) + 3</f>
-        <v>262.94674703153</v>
+        <v>107</v>
+      </c>
+      <c r="C108" s="1" t="n">
+        <v>107</v>
+      </c>
+      <c r="D108" s="1" t="n">
+        <f aca="true">2 * B108 + 3 + RAND()*(50-3) + 3</f>
+        <v>226.052079752088</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1110,8 +1764,14 @@
         <v>108</v>
       </c>
       <c r="B109" s="1" t="n">
-        <f aca="true">2 * A109 + 3 + RAND()*(50-3) + 3</f>
-        <v>238.771215464059</v>
+        <v>108</v>
+      </c>
+      <c r="C109" s="1" t="n">
+        <v>108</v>
+      </c>
+      <c r="D109" s="1" t="n">
+        <f aca="true">2 * B109 + 3 + RAND()*(50-3) + 3</f>
+        <v>253.657950561028</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1119,8 +1779,14 @@
         <v>109</v>
       </c>
       <c r="B110" s="1" t="n">
-        <f aca="true">2 * A110 + 3 + RAND()*(50-3) + 3</f>
-        <v>239.432706440789</v>
+        <v>109</v>
+      </c>
+      <c r="C110" s="1" t="n">
+        <v>109</v>
+      </c>
+      <c r="D110" s="1" t="n">
+        <f aca="true">2 * B110 + 3 + RAND()*(50-3) + 3</f>
+        <v>224.669528753962</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1128,8 +1794,14 @@
         <v>110</v>
       </c>
       <c r="B111" s="1" t="n">
-        <f aca="true">2 * A111 + 3 + RAND()*(50-3) + 3</f>
-        <v>229.301679714938</v>
+        <v>110</v>
+      </c>
+      <c r="C111" s="1" t="n">
+        <v>110</v>
+      </c>
+      <c r="D111" s="1" t="n">
+        <f aca="true">2 * B111 + 3 + RAND()*(50-3) + 3</f>
+        <v>259.788407459622</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1137,8 +1809,14 @@
         <v>111</v>
       </c>
       <c r="B112" s="1" t="n">
-        <f aca="true">2 * A112 + 3 + RAND()*(50-3) + 3</f>
-        <v>256.290929633745</v>
+        <v>111</v>
+      </c>
+      <c r="C112" s="1" t="n">
+        <v>111</v>
+      </c>
+      <c r="D112" s="1" t="n">
+        <f aca="true">2 * B112 + 3 + RAND()*(50-3) + 3</f>
+        <v>265.764627055963</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1146,8 +1824,14 @@
         <v>112</v>
       </c>
       <c r="B113" s="1" t="n">
-        <f aca="true">2 * A113 + 3 + RAND()*(50-3) + 3</f>
-        <v>235.581314661787</v>
+        <v>112</v>
+      </c>
+      <c r="C113" s="1" t="n">
+        <v>112</v>
+      </c>
+      <c r="D113" s="1" t="n">
+        <f aca="true">2 * B113 + 3 + RAND()*(50-3) + 3</f>
+        <v>262.206743810792</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1155,8 +1839,14 @@
         <v>113</v>
       </c>
       <c r="B114" s="1" t="n">
-        <f aca="true">2 * A114 + 3 + RAND()*(50-3) + 3</f>
-        <v>271.848052386295</v>
+        <v>113</v>
+      </c>
+      <c r="C114" s="1" t="n">
+        <v>113</v>
+      </c>
+      <c r="D114" s="1" t="n">
+        <f aca="true">2 * B114 + 3 + RAND()*(50-3) + 3</f>
+        <v>267.547362663085</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1164,8 +1854,14 @@
         <v>114</v>
       </c>
       <c r="B115" s="1" t="n">
-        <f aca="true">2 * A115 + 3 + RAND()*(50-3) + 3</f>
-        <v>272.947949417531</v>
+        <v>114</v>
+      </c>
+      <c r="C115" s="1" t="n">
+        <v>114</v>
+      </c>
+      <c r="D115" s="1" t="n">
+        <f aca="true">2 * B115 + 3 + RAND()*(50-3) + 3</f>
+        <v>269.362313817022</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1173,8 +1869,14 @@
         <v>115</v>
       </c>
       <c r="B116" s="1" t="n">
-        <f aca="true">2 * A116 + 3 + RAND()*(50-3) + 3</f>
-        <v>238.717471616173</v>
+        <v>115</v>
+      </c>
+      <c r="C116" s="1" t="n">
+        <v>115</v>
+      </c>
+      <c r="D116" s="1" t="n">
+        <f aca="true">2 * B116 + 3 + RAND()*(50-3) + 3</f>
+        <v>264.34995868965</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1182,8 +1884,14 @@
         <v>116</v>
       </c>
       <c r="B117" s="1" t="n">
-        <f aca="true">2 * A117 + 3 + RAND()*(50-3) + 3</f>
-        <v>251.063535362636</v>
+        <v>116</v>
+      </c>
+      <c r="C117" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="D117" s="1" t="n">
+        <f aca="true">2 * B117 + 3 + RAND()*(50-3) + 3</f>
+        <v>244.025962249609</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,8 +1899,14 @@
         <v>117</v>
       </c>
       <c r="B118" s="1" t="n">
-        <f aca="true">2 * A118 + 3 + RAND()*(50-3) + 3</f>
-        <v>248.671653805457</v>
+        <v>117</v>
+      </c>
+      <c r="C118" s="1" t="n">
+        <v>117</v>
+      </c>
+      <c r="D118" s="1" t="n">
+        <f aca="true">2 * B118 + 3 + RAND()*(50-3) + 3</f>
+        <v>254.449664094485</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1200,8 +1914,14 @@
         <v>118</v>
       </c>
       <c r="B119" s="1" t="n">
-        <f aca="true">2 * A119 + 3 + RAND()*(50-3) + 3</f>
-        <v>247.24996966775</v>
+        <v>118</v>
+      </c>
+      <c r="C119" s="1" t="n">
+        <v>118</v>
+      </c>
+      <c r="D119" s="1" t="n">
+        <f aca="true">2 * B119 + 3 + RAND()*(50-3) + 3</f>
+        <v>249.426558130421</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1209,8 +1929,14 @@
         <v>119</v>
       </c>
       <c r="B120" s="1" t="n">
-        <f aca="true">2 * A120 + 3 + RAND()*(50-3) + 3</f>
-        <v>249.926472533958</v>
+        <v>119</v>
+      </c>
+      <c r="C120" s="1" t="n">
+        <v>119</v>
+      </c>
+      <c r="D120" s="1" t="n">
+        <f aca="true">2 * B120 + 3 + RAND()*(50-3) + 3</f>
+        <v>281.622646886623</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1218,8 +1944,14 @@
         <v>120</v>
       </c>
       <c r="B121" s="1" t="n">
-        <f aca="true">2 * A121 + 3 + RAND()*(50-3) + 3</f>
-        <v>250.581749112511</v>
+        <v>120</v>
+      </c>
+      <c r="C121" s="1" t="n">
+        <v>120</v>
+      </c>
+      <c r="D121" s="1" t="n">
+        <f aca="true">2 * B121 + 3 + RAND()*(50-3) + 3</f>
+        <v>267.25197521341</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1227,8 +1959,14 @@
         <v>121</v>
       </c>
       <c r="B122" s="1" t="n">
-        <f aca="true">2 * A122 + 3 + RAND()*(50-3) + 3</f>
-        <v>266.036633913807</v>
+        <v>121</v>
+      </c>
+      <c r="C122" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="D122" s="1" t="n">
+        <f aca="true">2 * B122 + 3 + RAND()*(50-3) + 3</f>
+        <v>273.699984774226</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1236,8 +1974,14 @@
         <v>122</v>
       </c>
       <c r="B123" s="1" t="n">
-        <f aca="true">2 * A123 + 3 + RAND()*(50-3) + 3</f>
-        <v>283.940192710491</v>
+        <v>122</v>
+      </c>
+      <c r="C123" s="1" t="n">
+        <v>122</v>
+      </c>
+      <c r="D123" s="1" t="n">
+        <f aca="true">2 * B123 + 3 + RAND()*(50-3) + 3</f>
+        <v>260.120817030547</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1245,8 +1989,14 @@
         <v>123</v>
       </c>
       <c r="B124" s="1" t="n">
-        <f aca="true">2 * A124 + 3 + RAND()*(50-3) + 3</f>
-        <v>294.235058016999</v>
+        <v>123</v>
+      </c>
+      <c r="C124" s="1" t="n">
+        <v>123</v>
+      </c>
+      <c r="D124" s="1" t="n">
+        <f aca="true">2 * B124 + 3 + RAND()*(50-3) + 3</f>
+        <v>256.093657185556</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1254,8 +2004,14 @@
         <v>124</v>
       </c>
       <c r="B125" s="1" t="n">
-        <f aca="true">2 * A125 + 3 + RAND()*(50-3) + 3</f>
-        <v>300.602636747948</v>
+        <v>124</v>
+      </c>
+      <c r="C125" s="1" t="n">
+        <v>124</v>
+      </c>
+      <c r="D125" s="1" t="n">
+        <f aca="true">2 * B125 + 3 + RAND()*(50-3) + 3</f>
+        <v>255.721212055767</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1263,8 +2019,14 @@
         <v>125</v>
       </c>
       <c r="B126" s="1" t="n">
-        <f aca="true">2 * A126 + 3 + RAND()*(50-3) + 3</f>
-        <v>261.452015007218</v>
+        <v>125</v>
+      </c>
+      <c r="C126" s="1" t="n">
+        <v>125</v>
+      </c>
+      <c r="D126" s="1" t="n">
+        <f aca="true">2 * B126 + 3 + RAND()*(50-3) + 3</f>
+        <v>299.173881676747</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,8 +2034,14 @@
         <v>126</v>
       </c>
       <c r="B127" s="1" t="n">
-        <f aca="true">2 * A127 + 3 + RAND()*(50-3) + 3</f>
-        <v>266.726544286798</v>
+        <v>126</v>
+      </c>
+      <c r="C127" s="1" t="n">
+        <v>126</v>
+      </c>
+      <c r="D127" s="1" t="n">
+        <f aca="true">2 * B127 + 3 + RAND()*(50-3) + 3</f>
+        <v>271.838979263324</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1281,8 +2049,14 @@
         <v>127</v>
       </c>
       <c r="B128" s="1" t="n">
-        <f aca="true">2 * A128 + 3 + RAND()*(50-3) + 3</f>
-        <v>272.050668386204</v>
+        <v>127</v>
+      </c>
+      <c r="C128" s="1" t="n">
+        <v>127</v>
+      </c>
+      <c r="D128" s="1" t="n">
+        <f aca="true">2 * B128 + 3 + RAND()*(50-3) + 3</f>
+        <v>294.247557742055</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1290,8 +2064,14 @@
         <v>128</v>
       </c>
       <c r="B129" s="1" t="n">
-        <f aca="true">2 * A129 + 3 + RAND()*(50-3) + 3</f>
-        <v>292.639471498836</v>
+        <v>128</v>
+      </c>
+      <c r="C129" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="D129" s="1" t="n">
+        <f aca="true">2 * B129 + 3 + RAND()*(50-3) + 3</f>
+        <v>279.912476622034</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1299,8 +2079,14 @@
         <v>129</v>
       </c>
       <c r="B130" s="1" t="n">
-        <f aca="true">2 * A130 + 3 + RAND()*(50-3) + 3</f>
-        <v>279.163792090989</v>
+        <v>129</v>
+      </c>
+      <c r="C130" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="D130" s="1" t="n">
+        <f aca="true">2 * B130 + 3 + RAND()*(50-3) + 3</f>
+        <v>293.984904603334</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1308,8 +2094,14 @@
         <v>130</v>
       </c>
       <c r="B131" s="1" t="n">
-        <f aca="true">2 * A131 + 3 + RAND()*(50-3) + 3</f>
-        <v>288.419123209557</v>
+        <v>130</v>
+      </c>
+      <c r="C131" s="1" t="n">
+        <v>130</v>
+      </c>
+      <c r="D131" s="1" t="n">
+        <f aca="true">2 * B131 + 3 + RAND()*(50-3) + 3</f>
+        <v>290.167323983042</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1317,8 +2109,14 @@
         <v>131</v>
       </c>
       <c r="B132" s="1" t="n">
-        <f aca="true">2 * A132 + 3 + RAND()*(50-3) + 3</f>
-        <v>283.58693145352</v>
+        <v>131</v>
+      </c>
+      <c r="C132" s="1" t="n">
+        <v>131</v>
+      </c>
+      <c r="D132" s="1" t="n">
+        <f aca="true">2 * B132 + 3 + RAND()*(50-3) + 3</f>
+        <v>294.4146075428</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1326,8 +2124,14 @@
         <v>132</v>
       </c>
       <c r="B133" s="1" t="n">
-        <f aca="true">2 * A133 + 3 + RAND()*(50-3) + 3</f>
-        <v>276.102804710962</v>
+        <v>132</v>
+      </c>
+      <c r="C133" s="1" t="n">
+        <v>132</v>
+      </c>
+      <c r="D133" s="1" t="n">
+        <f aca="true">2 * B133 + 3 + RAND()*(50-3) + 3</f>
+        <v>301.884025663836</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1335,8 +2139,14 @@
         <v>133</v>
       </c>
       <c r="B134" s="1" t="n">
-        <f aca="true">2 * A134 + 3 + RAND()*(50-3) + 3</f>
-        <v>291.725596905317</v>
+        <v>133</v>
+      </c>
+      <c r="C134" s="1" t="n">
+        <v>133</v>
+      </c>
+      <c r="D134" s="1" t="n">
+        <f aca="true">2 * B134 + 3 + RAND()*(50-3) + 3</f>
+        <v>272.103334461572</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,8 +2154,14 @@
         <v>134</v>
       </c>
       <c r="B135" s="1" t="n">
-        <f aca="true">2 * A135 + 3 + RAND()*(50-3) + 3</f>
-        <v>309.98349314413</v>
+        <v>134</v>
+      </c>
+      <c r="C135" s="1" t="n">
+        <v>134</v>
+      </c>
+      <c r="D135" s="1" t="n">
+        <f aca="true">2 * B135 + 3 + RAND()*(50-3) + 3</f>
+        <v>314.776969036087</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,8 +2169,14 @@
         <v>135</v>
       </c>
       <c r="B136" s="1" t="n">
-        <f aca="true">2 * A136 + 3 + RAND()*(50-3) + 3</f>
-        <v>320.997197167649</v>
+        <v>135</v>
+      </c>
+      <c r="C136" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="D136" s="1" t="n">
+        <f aca="true">2 * B136 + 3 + RAND()*(50-3) + 3</f>
+        <v>319.829517912818</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1362,8 +2184,14 @@
         <v>136</v>
       </c>
       <c r="B137" s="1" t="n">
-        <f aca="true">2 * A137 + 3 + RAND()*(50-3) + 3</f>
-        <v>293.367261833118</v>
+        <v>136</v>
+      </c>
+      <c r="C137" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="D137" s="1" t="n">
+        <f aca="true">2 * B137 + 3 + RAND()*(50-3) + 3</f>
+        <v>299.663142989157</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1371,8 +2199,14 @@
         <v>137</v>
       </c>
       <c r="B138" s="1" t="n">
-        <f aca="true">2 * A138 + 3 + RAND()*(50-3) + 3</f>
-        <v>323.376839435454</v>
+        <v>137</v>
+      </c>
+      <c r="C138" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="D138" s="1" t="n">
+        <f aca="true">2 * B138 + 3 + RAND()*(50-3) + 3</f>
+        <v>317.998344876571</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1380,8 +2214,14 @@
         <v>138</v>
       </c>
       <c r="B139" s="1" t="n">
-        <f aca="true">2 * A139 + 3 + RAND()*(50-3) + 3</f>
-        <v>296.957126287107</v>
+        <v>138</v>
+      </c>
+      <c r="C139" s="1" t="n">
+        <v>138</v>
+      </c>
+      <c r="D139" s="1" t="n">
+        <f aca="true">2 * B139 + 3 + RAND()*(50-3) + 3</f>
+        <v>285.908695675898</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1389,8 +2229,14 @@
         <v>139</v>
       </c>
       <c r="B140" s="1" t="n">
-        <f aca="true">2 * A140 + 3 + RAND()*(50-3) + 3</f>
-        <v>289.236839114082</v>
+        <v>139</v>
+      </c>
+      <c r="C140" s="1" t="n">
+        <v>139</v>
+      </c>
+      <c r="D140" s="1" t="n">
+        <f aca="true">2 * B140 + 3 + RAND()*(50-3) + 3</f>
+        <v>312.337091917638</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1398,8 +2244,14 @@
         <v>140</v>
       </c>
       <c r="B141" s="1" t="n">
-        <f aca="true">2 * A141 + 3 + RAND()*(50-3) + 3</f>
-        <v>293.963841649288</v>
+        <v>140</v>
+      </c>
+      <c r="C141" s="1" t="n">
+        <v>140</v>
+      </c>
+      <c r="D141" s="1" t="n">
+        <f aca="true">2 * B141 + 3 + RAND()*(50-3) + 3</f>
+        <v>319.479971172987</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,8 +2259,14 @@
         <v>141</v>
       </c>
       <c r="B142" s="1" t="n">
-        <f aca="true">2 * A142 + 3 + RAND()*(50-3) + 3</f>
-        <v>312.341056093907</v>
+        <v>141</v>
+      </c>
+      <c r="C142" s="1" t="n">
+        <v>141</v>
+      </c>
+      <c r="D142" s="1" t="n">
+        <f aca="true">2 * B142 + 3 + RAND()*(50-3) + 3</f>
+        <v>312.439028609078</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,8 +2274,14 @@
         <v>142</v>
       </c>
       <c r="B143" s="1" t="n">
-        <f aca="true">2 * A143 + 3 + RAND()*(50-3) + 3</f>
-        <v>305.189391263756</v>
+        <v>142</v>
+      </c>
+      <c r="C143" s="1" t="n">
+        <v>142</v>
+      </c>
+      <c r="D143" s="1" t="n">
+        <f aca="true">2 * B143 + 3 + RAND()*(50-3) + 3</f>
+        <v>336.167184123769</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1425,8 +2289,14 @@
         <v>143</v>
       </c>
       <c r="B144" s="1" t="n">
-        <f aca="true">2 * A144 + 3 + RAND()*(50-3) + 3</f>
-        <v>316.642937357392</v>
+        <v>143</v>
+      </c>
+      <c r="C144" s="1" t="n">
+        <v>143</v>
+      </c>
+      <c r="D144" s="1" t="n">
+        <f aca="true">2 * B144 + 3 + RAND()*(50-3) + 3</f>
+        <v>323.588959890185</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1434,8 +2304,14 @@
         <v>144</v>
       </c>
       <c r="B145" s="1" t="n">
-        <f aca="true">2 * A145 + 3 + RAND()*(50-3) + 3</f>
-        <v>335.826619394344</v>
+        <v>144</v>
+      </c>
+      <c r="C145" s="1" t="n">
+        <v>144</v>
+      </c>
+      <c r="D145" s="1" t="n">
+        <f aca="true">2 * B145 + 3 + RAND()*(50-3) + 3</f>
+        <v>304.784750465769</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1443,8 +2319,14 @@
         <v>145</v>
       </c>
       <c r="B146" s="1" t="n">
-        <f aca="true">2 * A146 + 3 + RAND()*(50-3) + 3</f>
-        <v>307.877327016156</v>
+        <v>145</v>
+      </c>
+      <c r="C146" s="1" t="n">
+        <v>145</v>
+      </c>
+      <c r="D146" s="1" t="n">
+        <f aca="true">2 * B146 + 3 + RAND()*(50-3) + 3</f>
+        <v>342.09528854629</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1452,8 +2334,14 @@
         <v>146</v>
       </c>
       <c r="B147" s="1" t="n">
-        <f aca="true">2 * A147 + 3 + RAND()*(50-3) + 3</f>
-        <v>324.815459824291</v>
+        <v>146</v>
+      </c>
+      <c r="C147" s="1" t="n">
+        <v>146</v>
+      </c>
+      <c r="D147" s="1" t="n">
+        <f aca="true">2 * B147 + 3 + RAND()*(50-3) + 3</f>
+        <v>333.487306087278</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1461,8 +2349,14 @@
         <v>147</v>
       </c>
       <c r="B148" s="1" t="n">
-        <f aca="true">2 * A148 + 3 + RAND()*(50-3) + 3</f>
-        <v>304.508111178629</v>
+        <v>147</v>
+      </c>
+      <c r="C148" s="1" t="n">
+        <v>147</v>
+      </c>
+      <c r="D148" s="1" t="n">
+        <f aca="true">2 * B148 + 3 + RAND()*(50-3) + 3</f>
+        <v>324.469521576771</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1470,8 +2364,14 @@
         <v>148</v>
       </c>
       <c r="B149" s="1" t="n">
-        <f aca="true">2 * A149 + 3 + RAND()*(50-3) + 3</f>
-        <v>344.374822087591</v>
+        <v>148</v>
+      </c>
+      <c r="C149" s="1" t="n">
+        <v>148</v>
+      </c>
+      <c r="D149" s="1" t="n">
+        <f aca="true">2 * B149 + 3 + RAND()*(50-3) + 3</f>
+        <v>344.609911404084</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1479,8 +2379,14 @@
         <v>149</v>
       </c>
       <c r="B150" s="1" t="n">
-        <f aca="true">2 * A150 + 3 + RAND()*(50-3) + 3</f>
-        <v>346.419619747189</v>
+        <v>149</v>
+      </c>
+      <c r="C150" s="1" t="n">
+        <v>149</v>
+      </c>
+      <c r="D150" s="1" t="n">
+        <f aca="true">2 * B150 + 3 + RAND()*(50-3) + 3</f>
+        <v>304.909422421595</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1488,8 +2394,14 @@
         <v>150</v>
       </c>
       <c r="B151" s="1" t="n">
-        <f aca="true">2 * A151 + 3 + RAND()*(50-3) + 3</f>
-        <v>308.149449495382</v>
+        <v>150</v>
+      </c>
+      <c r="C151" s="1" t="n">
+        <v>150</v>
+      </c>
+      <c r="D151" s="1" t="n">
+        <f aca="true">2 * B151 + 3 + RAND()*(50-3) + 3</f>
+        <v>349.68049184815</v>
       </c>
     </row>
   </sheetData>

</xml_diff>